<commit_message>
Added the tasks for today
Added the tasks for today
</commit_message>
<xml_diff>
--- a/Documents/DataBase Table Structure.xlsx
+++ b/Documents/DataBase Table Structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rohan\Personal\Courses\Summer Of Code\SPDX\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rohan\Personal\Courses\Summer Of Code\SPDX\license-mgmt\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB779F3-2E5E-45AC-B06D-456DBCF502EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C869F5-F4DF-4A11-96EB-4AC76E95975D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="104">
   <si>
     <t>Column Name</t>
   </si>
@@ -370,6 +370,21 @@
   </si>
   <si>
     <t>Permission for group</t>
+  </si>
+  <si>
+    <t>Namespace</t>
+  </si>
+  <si>
+    <t>namespaceText</t>
+  </si>
+  <si>
+    <t>Varchar(30)</t>
+  </si>
+  <si>
+    <t>Namespace Text</t>
+  </si>
+  <si>
+    <t>Foreign key to namespace table</t>
   </si>
 </sst>
 </file>
@@ -968,17 +983,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.21875" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.5546875" customWidth="1"/>
     <col min="4" max="4" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1065,10 +1080,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>18</v>
@@ -1228,9 +1243,9 @@
       <c r="A23" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
@@ -1278,9 +1293,9 @@
       <c r="A29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
@@ -1328,9 +1343,9 @@
       <c r="A35" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
@@ -1378,9 +1393,9 @@
       <c r="A41" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
@@ -1512,9 +1527,9 @@
       <c r="A54" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
     </row>
     <row r="55" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
@@ -1590,9 +1605,9 @@
       <c r="A62" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
     </row>
     <row r="63" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
@@ -1650,8 +1665,59 @@
         <v>98</v>
       </c>
     </row>
+    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A69:D69"/>
     <mergeCell ref="A54:D54"/>
     <mergeCell ref="A62:D62"/>
     <mergeCell ref="A1:D1"/>

</xml_diff>